<commit_message>
Updated to latest V6 codelists
</commit_message>
<xml_diff>
--- a/peppol-id/src/test/resources/codelists/PEPPOL Code Lists - Document types v6 draft.xlsx
+++ b/peppol-id/src/test/resources/codelists/PEPPOL Code Lists - Document types v6 draft.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="18915" windowHeight="12300"/>
+    <workbookView xWindow="120" yWindow="110" windowWidth="18920" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Document Type" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Document Type'!$A$1:$J$69</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Document Type'!$A$1:$K$73</definedName>
     <definedName name="_ftn1" localSheetId="0">'Document Type'!#REF!</definedName>
     <definedName name="_ftn2" localSheetId="0">'Document Type'!#REF!</definedName>
     <definedName name="_ftn3" localSheetId="0">'Document Type'!#REF!</definedName>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="190">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -207,12 +207,6 @@
     <t>urn:oasis:names:specification:ubl:schema:xsd:Order-2::Order##urn:www.cenbii.eu:transaction:biitrns001:ver2.0:extended:urn:www.peppol.eu:bis:peppol3a:ver2.0::2.1</t>
   </si>
   <si>
-    <t>PEPPOL Identifier Scheme</t>
-  </si>
-  <si>
-    <t>PEPPOL Document Type Identifier</t>
-  </si>
-  <si>
     <t>busdox-docid-qns</t>
   </si>
   <si>
@@ -246,9 +240,6 @@
     <t>urn:oasis:names:specification:ubl:schema:xsd:CreditNote-2::CreditNote##urn:cen.eu:en16931:2017#conformant#urn:UBL.BE:1.0.0.20180214::2.1</t>
   </si>
   <si>
-    <t>Profile code</t>
-  </si>
-  <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:Order-2::Order##urn:www.cenbii.eu:transaction:biitrns001:ver2.0:extended:urn:www.peppol.eu:bis:peppol03a:ver2.0::2.1</t>
   </si>
   <si>
@@ -390,9 +381,6 @@
     <t>Procurement procedure subscription Request V1</t>
   </si>
   <si>
-    <t>DHSC Customized  Ordering profile OrderResponse V1</t>
-  </si>
-  <si>
     <t>DHSC Customized Ordering profile Order V1</t>
   </si>
   <si>
@@ -468,9 +456,6 @@
     <t>POAC</t>
   </si>
   <si>
-    <t>Issued OpenPEPPOL?</t>
-  </si>
-  <si>
     <t>AU-NZ Self-Billing 3.0 Invoice</t>
   </si>
   <si>
@@ -493,6 +478,126 @@
   </si>
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:CreditNote-2::CreditNote##urn:cen.eu:en16931:2017#conformant#urn:fdc:peppol.eu:2017:poacc:selfbilling:international:aunz:3.0::2.1</t>
+  </si>
+  <si>
+    <t>Profile name</t>
+  </si>
+  <si>
+    <t>Issued by OpenPEPPOL?</t>
+  </si>
+  <si>
+    <t>DHSC Customized Ordering profile OrderResponse V1</t>
+  </si>
+  <si>
+    <t>Peppol Document Type Identifier Scheme</t>
+  </si>
+  <si>
+    <t>Peppol Document Type Identifier Value</t>
+  </si>
+  <si>
+    <t>Associated Process Identifier(s)</t>
+  </si>
+  <si>
+    <t>oioubl-procid-ubl::Reference-Utility-1.0</t>
+  </si>
+  <si>
+    <t>oioubl-procid-ubl::Procurement-ReminderOnly-1.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:peppol.eu:2017:poacc:billing:01:1.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:www.peppol.eu:profile:bis63a:ver1.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:peppol.eu:poacc:bis:catalogue_only:3
+cenbii-procid-ubl::urn:fdc:peppol.eu:poacc:bis:catalogue_wo_response:3</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:peppol.eu:poacc:bis:catalogue_only:3</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:peppol.eu:poacc:bis:ordering:3
+cenbii-procid-ubl::urn:fdc:peppol.eu:poacc:bis:order_only:3</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:peppol.eu:poacc:bis:invoice_response:3</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:peppol.eu:poacc:bis:punch_out:3</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:peppol.eu:poacc:bis:ordering:3</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:peppol.eu:poacc:bis:despatch_advice:3</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:peppol.eu:poacc:bis:order_agreement:3</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:peppol.eu:poacc:bis:mlr:3</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:www.efaktura.gov.pl:ver1.0:account_corr:ver1.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:www.efaktura.gov.pl:ver1.0:corr_inv:ver1.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:www.efaktura.gov.pl:ver1.0:receipt_advice:ver1.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:peppol.eu:2017:pracc:p003:01:1.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:peppol.eu:2017:pracc:p002:01:1.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:peppol.eu:2017:pracc:p001:01:1.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::none</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:www.cenbii.eu:profile:bii01:ver1.0
+cenbii-procid-ubl::urn:www.cenbii.eu:profile:bii01:ver2.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:www.cenbii.eu:profile:bii01:ver1.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:www.cenbii.eu:profile:bii01:ver2.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:www.cenbii.eu:profile:bii03:ver1.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:www.cenbii.eu:profile:bii03:ver2.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:www.cenbii.eu:profile:bii04:ver1.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:www.cenbii.eu:profile:bii04:ver2.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:www.cenbii.eu:profile:bii05:ver1.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:www.cenbii.eu:profile:bii05:ver2.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:www.cenbii.eu:profile:bii06:ver1.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:www.cenbii.eu:profile:bii28:ver2.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:www.cenbii.eu:profile:bii30:ver2.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:www.cenbii.eu:profile:bii36:ver2.0</t>
   </si>
 </sst>
 </file>
@@ -558,7 +663,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -581,8 +686,11 @@
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -983,35 +1091,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J73"/>
+  <dimension ref="A1:K73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A71" sqref="A71"/>
+    <sheetView tabSelected="1" topLeftCell="D24" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.36328125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="47.59765625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" style="4" customWidth="1"/>
-    <col min="3" max="3" width="103.1328125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="47.6328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.26953125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="103.08984375" style="4" customWidth="1"/>
     <col min="4" max="4" width="8" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.59765625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.73046875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.59765625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.86328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="11.3984375" style="4"/>
+    <col min="5" max="5" width="14.6328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.81640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="11.36328125" style="4"/>
+    <col min="11" max="11" width="64.90625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="11.36328125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="28.5">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="29">
       <c r="A1" s="1" t="s">
-        <v>73</v>
+        <v>151</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>154</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>61</v>
+        <v>155</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>16</v>
@@ -1023,24 +1132,27 @@
         <v>45</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="42.75">
+        <v>140</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="43.5">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>12</v>
@@ -1063,15 +1175,18 @@
         <v>1</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="42.75">
+        <v>141</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="43.5">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>13</v>
@@ -1094,15 +1209,18 @@
         <v>1</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="28.5">
+        <v>141</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="43.5">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>14</v>
@@ -1125,15 +1243,18 @@
         <v>1</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="28.5">
+        <v>141</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="29">
       <c r="A5" s="4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>22</v>
@@ -1156,15 +1277,18 @@
         <v>1</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="43.5">
       <c r="A6" s="4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>0</v>
@@ -1187,15 +1311,18 @@
         <v>1</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="43.5">
       <c r="A7" s="4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>1</v>
@@ -1218,15 +1345,18 @@
         <v>1</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="29">
       <c r="A8" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>32</v>
@@ -1246,15 +1376,18 @@
         <v>1</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="29">
       <c r="A9" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>15</v>
@@ -1277,18 +1410,21 @@
         <v>1</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="29">
       <c r="A10" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>28</v>
@@ -1311,15 +1447,18 @@
         <v>2</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="29">
       <c r="A11" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>59</v>
@@ -1339,15 +1478,18 @@
         <v>2</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="29">
       <c r="A12" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>2</v>
@@ -1370,15 +1512,18 @@
         <v>1</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="29">
       <c r="A13" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>31</v>
@@ -1398,15 +1543,18 @@
         <v>2</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="29">
       <c r="A14" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>19</v>
@@ -1429,15 +1577,18 @@
         <v>1</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="29">
       <c r="A15" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>20</v>
@@ -1460,15 +1611,18 @@
         <v>1</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="29">
       <c r="A16" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>21</v>
@@ -1491,15 +1645,18 @@
         <v>1</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="29">
       <c r="A17" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>33</v>
@@ -1519,15 +1676,18 @@
         <v>2</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="29">
       <c r="A18" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>34</v>
@@ -1547,15 +1707,18 @@
         <v>2</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="29">
       <c r="A19" s="4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>3</v>
@@ -1575,15 +1738,18 @@
         <v>1</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="43.5">
       <c r="A20" s="4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>10</v>
@@ -1603,15 +1769,18 @@
         <v>1</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="43.5">
       <c r="A21" s="4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>11</v>
@@ -1631,15 +1800,18 @@
         <v>1</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="29">
       <c r="A22" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>4</v>
@@ -1659,15 +1831,18 @@
         <v>1</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="29">
       <c r="A23" s="4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>5</v>
@@ -1687,15 +1862,18 @@
         <v>1</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="29">
       <c r="A24" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>6</v>
@@ -1715,15 +1893,18 @@
         <v>1</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="42.75">
+        <v>142</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="43.5">
       <c r="A25" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>23</v>
@@ -1743,15 +1924,18 @@
         <v>0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="42.75">
+        <v>142</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="43.5">
       <c r="A26" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>25</v>
@@ -1768,15 +1952,18 @@
         <v>0</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="29">
       <c r="A27" s="4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>38</v>
@@ -1796,15 +1983,18 @@
         <v>1</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="29">
       <c r="A28" s="4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>39</v>
@@ -1829,15 +2019,18 @@
         <v>1</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="43.5">
       <c r="A29" s="4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>50</v>
@@ -1857,15 +2050,18 @@
         <v>1</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="43.5">
       <c r="A30" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>42</v>
@@ -1885,15 +2081,18 @@
         <v>1</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="42.75">
+        <v>142</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="43.5">
       <c r="A31" s="4" t="s">
         <v>41</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>43</v>
@@ -1913,15 +2112,18 @@
         <v>1</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K31" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="29">
       <c r="A32" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>46</v>
@@ -1941,15 +2143,18 @@
         <v>3</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K32" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="29">
       <c r="A33" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>47</v>
@@ -1969,15 +2174,18 @@
         <v>3</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="42.75">
+        <v>142</v>
+      </c>
+      <c r="K33" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="43.5">
       <c r="A34" s="4" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>48</v>
@@ -1994,15 +2202,18 @@
         <v>0</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="42.75">
+        <v>142</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="43.5">
       <c r="A35" s="4" t="s">
-        <v>121</v>
+        <v>153</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>49</v>
@@ -2019,15 +2230,18 @@
         <v>0</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="29">
       <c r="A36" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>52</v>
@@ -2047,15 +2261,18 @@
         <v>3</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="42.75">
+        <v>142</v>
+      </c>
+      <c r="K36" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="43.5">
       <c r="A37" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>53</v>
@@ -2075,15 +2292,18 @@
         <v>1</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="42.75">
+        <v>141</v>
+      </c>
+      <c r="K37" s="4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="43.5">
       <c r="A38" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>54</v>
@@ -2103,15 +2323,18 @@
         <v>1</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="42.75">
+        <v>141</v>
+      </c>
+      <c r="K38" s="4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="43.5">
       <c r="A39" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>55</v>
@@ -2131,15 +2354,18 @@
         <v>1</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="28.5">
+        <v>141</v>
+      </c>
+      <c r="K39" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="43.5">
       <c r="A40" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>56</v>
@@ -2159,15 +2385,18 @@
         <v>1</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="28.5">
+        <v>141</v>
+      </c>
+      <c r="K40" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="43.5">
       <c r="A41" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>57</v>
@@ -2187,15 +2416,18 @@
         <v>1</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="28.5">
+        <v>141</v>
+      </c>
+      <c r="K41" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="29">
       <c r="A42" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>58</v>
@@ -2215,18 +2447,21 @@
         <v>1</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="28.5">
+        <v>141</v>
+      </c>
+      <c r="K42" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="29">
       <c r="A43" s="4" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D43" s="4">
         <v>3</v>
@@ -2242,18 +2477,21 @@
         <v>0</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K43" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="29">
       <c r="A44" s="4" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B44" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>64</v>
       </c>
       <c r="D44" s="4">
         <v>3</v>
@@ -2269,18 +2507,21 @@
         <v>0</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K44" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="29">
       <c r="A45" s="4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D45" s="4">
         <v>3</v>
@@ -2296,94 +2537,106 @@
         <v>0</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10">
+        <v>142</v>
+      </c>
+      <c r="K45" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
       <c r="A46" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D46" s="4">
+        <v>3</v>
+      </c>
+      <c r="E46" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H46" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="J46" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="K46" s="8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="A47" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D47" s="4">
+        <v>3</v>
+      </c>
+      <c r="E47" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H47" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="J47" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="K47" s="8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="29">
+      <c r="A48" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D46" s="4">
-        <v>3</v>
-      </c>
-      <c r="E46" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="H46" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="J46" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10">
-      <c r="A47" s="4" t="s">
+      <c r="B48" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D48" s="4">
+        <v>3</v>
+      </c>
+      <c r="E48" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H48" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="J48" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="K48" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="29">
+      <c r="A49" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D47" s="4">
-        <v>3</v>
-      </c>
-      <c r="E47" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="H47" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="J47" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="28.5">
-      <c r="A48" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D48" s="4">
-        <v>3</v>
-      </c>
-      <c r="E48" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="H48" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="J48" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="28.5">
-      <c r="A49" s="4" t="s">
+      <c r="B49" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C49" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>72</v>
-      </c>
       <c r="D49" s="4">
         <v>3</v>
       </c>
@@ -2396,18 +2649,21 @@
         <v>0</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K49" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="29">
       <c r="A50" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D50" s="4">
         <v>4</v>
@@ -2424,18 +2680,21 @@
         <v>1</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10">
+        <v>142</v>
+      </c>
+      <c r="K50" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="29">
       <c r="A51" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D51" s="4">
         <v>4</v>
@@ -2452,18 +2711,21 @@
         <v>3</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K51" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="29">
       <c r="A52" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D52" s="4">
         <v>4</v>
@@ -2480,18 +2742,21 @@
         <v>3</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10">
+        <v>142</v>
+      </c>
+      <c r="K52" s="8" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="29">
       <c r="A53" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D53" s="4">
         <v>4</v>
@@ -2508,18 +2773,21 @@
         <v>3</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K53" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="29">
       <c r="A54" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D54" s="4">
         <v>4</v>
@@ -2536,18 +2804,21 @@
         <v>3</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10">
+        <v>142</v>
+      </c>
+      <c r="K54" s="8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
       <c r="A55" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D55" s="4">
         <v>4</v>
@@ -2564,18 +2835,21 @@
         <v>3</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K55" s="8" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="29">
       <c r="A56" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D56" s="4">
         <v>4</v>
@@ -2592,18 +2866,21 @@
         <v>3</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K56" s="8" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="29">
       <c r="A57" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D57" s="4">
         <v>4</v>
@@ -2620,18 +2897,21 @@
         <v>3</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K57" s="8" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="29">
       <c r="A58" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D58" s="4">
         <v>4</v>
@@ -2648,18 +2928,21 @@
         <v>3</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K58" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="29">
       <c r="A59" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D59" s="4">
         <v>4</v>
@@ -2676,18 +2959,21 @@
         <v>3</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K59" s="8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="29">
       <c r="A60" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D60" s="4">
         <v>4</v>
@@ -2701,18 +2987,21 @@
         <v>0</v>
       </c>
       <c r="J60" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K60" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="29">
       <c r="A61" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D61" s="4">
         <v>4</v>
@@ -2726,18 +3015,21 @@
         <v>0</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" ht="28.5">
-      <c r="A62" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="K61" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="29">
+      <c r="A62" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C62" s="4" t="s">
         <v>100</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>103</v>
       </c>
       <c r="D62" s="4">
         <v>4</v>
@@ -2754,18 +3046,21 @@
         <v>3</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K62" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" ht="29">
       <c r="A63" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D63" s="4">
         <v>4</v>
@@ -2782,18 +3077,21 @@
         <v>3</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K63" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="29">
       <c r="A64" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C64" s="4" t="s">
         <v>104</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>107</v>
       </c>
       <c r="D64" s="4">
         <v>5</v>
@@ -2807,18 +3105,21 @@
         <v>0</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K64" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" ht="29">
       <c r="A65" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C65" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>108</v>
       </c>
       <c r="D65" s="4">
         <v>5</v>
@@ -2832,18 +3133,21 @@
         <v>0</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K65" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" ht="29">
       <c r="A66" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C66" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>109</v>
       </c>
       <c r="D66" s="4">
         <v>5</v>
@@ -2857,18 +3161,21 @@
         <v>0</v>
       </c>
       <c r="J66" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K66" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" ht="29">
       <c r="A67" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C67" s="4" t="s">
         <v>136</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>140</v>
       </c>
       <c r="D67" s="4">
         <v>6</v>
@@ -2882,18 +3189,21 @@
         <v>0</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" ht="42.75">
+        <v>142</v>
+      </c>
+      <c r="K67" s="8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" ht="43.5">
       <c r="A68" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D68" s="4">
         <v>6</v>
@@ -2907,18 +3217,21 @@
         <v>0</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K68" s="8" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" ht="29">
       <c r="A69" s="4" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D69" s="4">
         <v>6</v>
@@ -2932,18 +3245,21 @@
         <v>0</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" ht="28.5">
-      <c r="A70" s="8" t="s">
-        <v>150</v>
+        <v>142</v>
+      </c>
+      <c r="K69" s="8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" ht="29">
+      <c r="A70" s="9" t="s">
+        <v>145</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="D70" s="4">
         <v>6</v>
@@ -2960,18 +3276,21 @@
         <v>3</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" ht="28.5">
-      <c r="A71" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="K70" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" ht="29">
+      <c r="A71" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C71" s="4" t="s">
         <v>149</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>154</v>
       </c>
       <c r="D71" s="4">
         <v>6</v>
@@ -2988,18 +3307,21 @@
         <v>3</v>
       </c>
       <c r="J71" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K71" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" ht="29">
       <c r="A72" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C72" s="4" t="s">
         <v>148</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>153</v>
       </c>
       <c r="D72" s="4">
         <v>6</v>
@@ -3013,18 +3335,21 @@
         <v>0</v>
       </c>
       <c r="J72" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="K72" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" ht="43.5">
+      <c r="A73" s="4" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="73" spans="1:10" ht="28.5">
-      <c r="A73" s="4" t="s">
-        <v>151</v>
-      </c>
       <c r="B73" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D73" s="4">
         <v>6</v>
@@ -3038,13 +3363,14 @@
         <v>0</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>146</v>
+        <v>142</v>
+      </c>
+      <c r="K73" s="8" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J69">
-    <filterColumn colId="9"/>
-  </autoFilter>
+  <autoFilter ref="A1:K73"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>